<commit_message>
updated to test ADO pipeline
</commit_message>
<xml_diff>
--- a/INPUT TEMPLATES/filebeat_input.xlsx
+++ b/INPUT TEMPLATES/filebeat_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://docs.philips.com/personal/ananyak_s_philips_com/Documents/Saved Pictures/filebeat generator 02/INPUT TEMPLATES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="186" documentId="11_AD4DB114E441178AC67DF4BEEE14EB98693EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B142BD0-F4F7-4252-8A77-0A7199E4C932}"/>
+  <xr:revisionPtr revIDLastSave="187" documentId="11_AD4DB114E441178AC67DF4BEEE14EB98693EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C5FD815-06B3-40DD-AA89-FE4B5B123879}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,9 +39,6 @@
     <t>request url</t>
   </si>
   <si>
-    <t xml:space="preserve">username </t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -106,6 +103,9 @@
   </si>
   <si>
     <t>partner id</t>
+  </si>
+  <si>
+    <t>username</t>
   </si>
 </sst>
 </file>
@@ -592,7 +592,7 @@
   <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -618,7 +618,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -629,7 +629,7 @@
       <c r="H1" s="11"/>
       <c r="I1" s="12"/>
       <c r="J1" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K1" s="18"/>
       <c r="L1" s="18"/>
@@ -654,11 +654,11 @@
       <c r="F2" s="13"/>
       <c r="G2" s="14"/>
       <c r="H2" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K2" s="16"/>
       <c r="L2" s="16"/>
@@ -671,7 +671,7 @@
       <c r="S2" s="16"/>
       <c r="T2" s="17"/>
       <c r="U2" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="V2" s="9"/>
       <c r="W2" s="8"/>
@@ -690,61 +690,61 @@
         <v>3</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="H3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="J3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="R3" s="5" t="s">
+      <c r="S3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="S3" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="T3" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="V3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="V3" s="5" t="s">
+      <c r="W3" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="W3" s="5" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>